<commit_message>
PAS-730: Auto CA select cases covered
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_CA_SELECT.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/AddedVIN_CA_SELECT.xlsx
@@ -258,9 +258,6 @@
     <t>4WD</t>
   </si>
   <si>
-    <t>9MSRP17H&amp;V</t>
-  </si>
-  <si>
     <t>VOLKSWAGEN</t>
   </si>
   <si>
@@ -271,13 +268,16 @@
   </si>
   <si>
     <t>RT</t>
+  </si>
+  <si>
+    <t>7MSRP15H&amp;V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,12 +306,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.4"/>
-      <color theme="1"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
@@ -325,7 +319,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -335,12 +329,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -357,7 +345,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -365,12 +353,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -654,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AE12" sqref="AE12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1254,117 +1236,116 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="15" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>66</v>
+    <row r="6" spans="1:38" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>2015</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="H6" s="4">
+        <v>88888</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="K6" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="H6" s="3">
-        <v>88888</v>
-      </c>
-      <c r="I6" s="3" t="s">
+      <c r="L6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="M6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J6" t="s">
+      <c r="N6" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="O6" s="4">
+        <v>12</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>214</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="S6" s="4">
+        <v>4</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="V6" s="4">
+        <v>2</v>
+      </c>
+      <c r="W6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="X6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z6" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="L6" t="s">
-        <v>69</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="O6" s="3">
-        <v>12</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q6" s="3">
-        <v>214</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="S6" s="3">
-        <v>4</v>
-      </c>
-      <c r="T6" s="3" t="s">
+      <c r="AA6" s="4">
         <v>33</v>
       </c>
-      <c r="U6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="V6" s="3">
-        <v>2</v>
-      </c>
-      <c r="W6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="X6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z6" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA6" s="6">
-        <v>33</v>
-      </c>
-      <c r="AB6" s="6">
+      <c r="AB6" s="4">
         <v>43</v>
       </c>
-      <c r="AC6" s="3"/>
-      <c r="AD6" s="3" t="s">
+      <c r="AD6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AE6" s="3" t="s">
+      <c r="AE6" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AF6" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="AG6" s="3" t="s">
+      <c r="AG6" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AH6" s="3" t="s">
+      <c r="AH6" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="AI6" s="3">
+      <c r="AI6" s="4">
         <v>20000101</v>
       </c>
-      <c r="AJ6" s="3" t="s">
+      <c r="AJ6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AK6" s="3" t="s">
+      <c r="AK6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AL6" s="3" t="s">
+      <c r="AL6" s="4" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>